<commit_message>
updated project timescale (during meeting) and added database details w/ Tassos
</commit_message>
<xml_diff>
--- a/Documentation/Design/Project Timescale.xlsx
+++ b/Documentation/Design/Project Timescale.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Sprint 0</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>Sprint effort</t>
+  </si>
+  <si>
+    <t>Basic functionality</t>
   </si>
 </sst>
 </file>
@@ -523,17 +526,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="36.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
@@ -613,7 +617,9 @@
         <v>34</v>
       </c>
       <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -662,6 +668,7 @@
         <v>2</v>
       </c>
       <c r="F8" s="2"/>
+      <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
@@ -733,6 +740,7 @@
       <c r="B16">
         <v>2</v>
       </c>
+      <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -829,22 +837,16 @@
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G26" s="7">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H26" s="7">
+        <v>16</v>
+      </c>
+      <c r="I26" s="7">
         <v>17</v>
-      </c>
-      <c r="I26" s="7">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B27">
-        <f>B26/4</f>
-        <v>15.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed dummyfile fixed some formatting in timescale
</commit_message>
<xml_diff>
--- a/Documentation/Design/Project Timescale.xlsx
+++ b/Documentation/Design/Project Timescale.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12945"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -529,18 +529,19 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
@@ -569,7 +570,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
@@ -604,7 +605,7 @@
         <v>42716</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>33</v>
       </c>
@@ -622,7 +623,7 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -632,7 +633,7 @@
       <c r="F4" s="8"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -642,7 +643,7 @@
       <c r="F5" s="8"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -651,7 +652,7 @@
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -660,7 +661,7 @@
       </c>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
@@ -670,7 +671,7 @@
       <c r="F8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -679,7 +680,7 @@
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
@@ -688,7 +689,7 @@
       </c>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
@@ -697,7 +698,7 @@
       </c>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
@@ -706,7 +707,7 @@
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
@@ -715,7 +716,7 @@
       </c>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
@@ -724,7 +725,7 @@
       </c>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
@@ -733,7 +734,7 @@
       </c>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>21</v>
       </c>
@@ -743,7 +744,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>22</v>
       </c>
@@ -752,7 +753,7 @@
       </c>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
@@ -762,7 +763,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="8"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>24</v>
       </c>
@@ -771,7 +772,7 @@
       </c>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>32</v>
       </c>
@@ -780,7 +781,7 @@
       </c>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>25</v>
       </c>
@@ -789,7 +790,7 @@
       </c>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>26</v>
       </c>
@@ -798,7 +799,7 @@
       </c>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
@@ -807,7 +808,7 @@
       </c>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>28</v>
       </c>
@@ -816,7 +817,7 @@
       </c>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>29</v>
       </c>
@@ -825,7 +826,7 @@
       </c>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
[multi] Updated my diary Added salt to Player table Added interfaces for the repositories (for unit testing) Added salt to Player model Implemented AuthenticationService
</commit_message>
<xml_diff>
--- a/Documentation/Design/Project Timescale.xlsx
+++ b/Documentation/Design/Project Timescale.xlsx
@@ -528,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,7 +538,7 @@
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>